<commit_message>
linearizing code, refactoring and reorganizing
</commit_message>
<xml_diff>
--- a/WF1_template.xlsx
+++ b/WF1_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F39B14B-5BE0-6D40-9175-91BD869AF4A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BF4ECA-74D6-704A-AA20-181D9A4A2527}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18840" yWindow="460" windowWidth="27880" windowHeight="27640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="500" windowWidth="27880" windowHeight="27640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WF1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="139">
   <si>
     <t>ExpWorkflowVer</t>
   </si>
@@ -430,10 +430,13 @@
     <t>FAH</t>
   </si>
   <si>
-    <t>AcNH3I</t>
-  </si>
-  <si>
     <t>Symyx_96_well_0003</t>
+  </si>
+  <si>
+    <t>PyrrolidiniumIodide</t>
+  </si>
+  <si>
+    <t>DMSO</t>
   </si>
 </sst>
 </file>
@@ -896,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1027,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="8">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>62</v>
@@ -1080,9 +1083,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
-        <v>49</v>
-      </c>
+      <c r="A10" s="44"/>
       <c r="B10" s="8" t="s">
         <v>94</v>
       </c>
@@ -1102,9 +1103,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
-        <v>49</v>
-      </c>
+      <c r="A11" s="44"/>
       <c r="B11" s="8" t="s">
         <v>46</v>
       </c>
@@ -1121,9 +1120,7 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="44" t="s">
-        <v>49</v>
-      </c>
+      <c r="A12" s="44"/>
       <c r="B12" s="8" t="s">
         <v>50</v>
       </c>
@@ -1140,9 +1137,7 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
-        <v>49</v>
-      </c>
+      <c r="A13" s="44"/>
       <c r="B13" s="8" t="s">
         <v>51</v>
       </c>
@@ -1159,9 +1154,7 @@
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
-        <v>49</v>
-      </c>
+      <c r="A14" s="44"/>
       <c r="B14" s="8" t="s">
         <v>52</v>
       </c>
@@ -1178,9 +1171,7 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="44" t="s">
-        <v>49</v>
-      </c>
+      <c r="A15" s="44"/>
       <c r="B15" s="8" t="s">
         <v>53</v>
       </c>
@@ -1197,9 +1188,7 @@
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="44" t="s">
-        <v>49</v>
-      </c>
+      <c r="A16" s="44"/>
       <c r="B16" s="8" t="s">
         <v>95</v>
       </c>
@@ -1283,7 +1272,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>60</v>
@@ -1389,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>60</v>
@@ -1457,9 +1446,7 @@
       <c r="G30" s="22"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="45" t="s">
-        <v>49</v>
-      </c>
+      <c r="A31" s="45"/>
       <c r="B31" s="23" t="s">
         <v>71</v>
       </c>
@@ -1680,7 +1667,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="23">
-        <v>1.5</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="E44" s="23" t="s">
         <v>63</v>
@@ -1699,7 +1686,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="23">
-        <v>0.56999999999999995</v>
+        <v>2.85</v>
       </c>
       <c r="E45" s="23" t="s">
         <v>63</v>
@@ -1803,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="23">
-        <v>6</v>
+        <v>4.18</v>
       </c>
       <c r="E51" s="23" t="s">
         <v>63</v>
@@ -1823,9 +1810,7 @@
       <c r="G52" s="22"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="45" t="s">
-        <v>49</v>
-      </c>
+      <c r="A53" s="45"/>
       <c r="B53" s="23" t="s">
         <v>114</v>
       </c>
@@ -1895,9 +1880,7 @@
       <c r="G56" s="22"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="45" t="s">
-        <v>49</v>
-      </c>
+      <c r="A57" s="45"/>
       <c r="B57" s="23" t="s">
         <v>116</v>
       </c>
@@ -2208,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E74" s="38" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Closes #7 work toward #5
</commit_message>
<xml_diff>
--- a/WF1_template.xlsx
+++ b/WF1_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BF4ECA-74D6-704A-AA20-181D9A4A2527}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6A2CB6-B909-D643-995E-DE849F16F46B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="500" windowWidth="27880" windowHeight="27640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="141">
   <si>
     <t>ExpWorkflowVer</t>
   </si>
@@ -28,9 +28,6 @@
     <t>=</t>
   </si>
   <si>
-    <t>The workflow version of the experimental protocol</t>
-  </si>
-  <si>
     <t xml:space="preserve"> number of experimental wells to dedicate to a particular experiment</t>
   </si>
   <si>
@@ -437,6 +434,15 @@
   </si>
   <si>
     <t>DMSO</t>
+  </si>
+  <si>
+    <t>This interface does not support specification of more than 9 experiments</t>
+  </si>
+  <si>
+    <t>Number of wells allocated to exp1 template (must be identical to 'wellcount' if the only experiment type on tray)</t>
+  </si>
+  <si>
+    <t>The workflow version of the experimental protocol.  Currently supported: 1, 1.1, 3</t>
   </si>
 </sst>
 </file>
@@ -899,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -915,30 +921,30 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="E1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="12"/>
@@ -959,19 +965,19 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>2</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
       <c r="B4" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>1</v>
@@ -980,51 +986,53 @@
         <v>0</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="19">
         <v>1</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="43"/>
       <c r="B5" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="44"/>
       <c r="B7" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>1</v>
@@ -1033,113 +1041,121 @@
         <v>96</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" s="8">
         <v>96</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="44"/>
       <c r="B8" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="44"/>
       <c r="B9" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="44"/>
       <c r="B10" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="8">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>139</v>
+      </c>
       <c r="H10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
+      <c r="A11" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="B11" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
+      <c r="A12" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="B12" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
+      <c r="A13" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="B13" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>1</v>
@@ -1148,59 +1164,64 @@
         <v>40</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
+      <c r="A14" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="B14" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
+      <c r="A15" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="B15" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
+      <c r="A16" s="44" t="s">
+        <v>48</v>
+      </c>
       <c r="B16" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="8">
-        <f>36</f>
         <v>36</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="6"/>
@@ -1208,7 +1229,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="44"/>
       <c r="B17" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>1</v>
@@ -1217,17 +1238,17 @@
         <v>500</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="44"/>
       <c r="B18" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>1</v>
@@ -1236,16 +1257,16 @@
         <v>750</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="24"/>
@@ -1266,22 +1287,22 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="45"/>
       <c r="B21" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1296,30 +1317,30 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="45"/>
       <c r="B23" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>1</v>
@@ -1328,21 +1349,21 @@
         <v>0.2</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F24" s="23">
         <v>0.1</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C25" s="24" t="s">
         <v>1</v>
@@ -1351,13 +1372,13 @@
         <v>1.5</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F25" s="28">
         <v>3</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1372,30 +1393,30 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="45"/>
       <c r="B27" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F27" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>1</v>
@@ -1404,21 +1425,21 @@
         <v>0</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F28" s="28">
         <v>3</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="24" t="s">
         <v>1</v>
@@ -1427,13 +1448,13 @@
         <v>4</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F29" s="28">
         <v>4</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1448,30 +1469,30 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="45"/>
       <c r="B31" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G31" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>1</v>
@@ -1480,21 +1501,21 @@
         <v>0</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F32" s="28">
         <v>3</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="24" t="s">
         <v>1</v>
@@ -1503,13 +1524,13 @@
         <v>4</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="28">
         <v>4</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1529,32 +1550,32 @@
       <c r="E35" s="23"/>
       <c r="F35" s="23"/>
       <c r="G35" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="45"/>
       <c r="B36" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
       <c r="G36" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C37" s="24" t="s">
         <v>1</v>
@@ -1563,19 +1584,19 @@
         <v>0</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F37" s="23"/>
       <c r="G37" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" s="31" t="s">
         <v>1</v>
@@ -1584,16 +1605,16 @@
         <v>5.5</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F38" s="30"/>
       <c r="G38" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="23"/>
       <c r="C39" s="24"/>
@@ -1614,20 +1635,20 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="45"/>
       <c r="B41" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>105</v>
-      </c>
       <c r="E41" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F41" s="23"/>
       <c r="G41" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1642,26 +1663,26 @@
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="45"/>
       <c r="B43" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C43" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" s="23" t="s">
-        <v>107</v>
-      </c>
       <c r="E43" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F43" s="23"/>
       <c r="G43" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="45"/>
       <c r="B44" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C44" s="25" t="s">
         <v>1</v>
@@ -1670,17 +1691,17 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F44" s="23"/>
       <c r="G44" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="45"/>
       <c r="B45" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C45" s="25" t="s">
         <v>1</v>
@@ -1689,19 +1710,19 @@
         <v>2.85</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F45" s="23"/>
       <c r="G45" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" s="24" t="s">
         <v>1</v>
@@ -1710,17 +1731,17 @@
         <v>75</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>1</v>
@@ -1729,17 +1750,17 @@
         <v>450</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F47" s="22"/>
       <c r="G47" s="22"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>1</v>
@@ -1748,7 +1769,7 @@
         <v>3600</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
@@ -1765,26 +1786,26 @@
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="45"/>
       <c r="B50" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="23" t="s">
-        <v>112</v>
-      </c>
       <c r="E50" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F50" s="23"/>
       <c r="G50" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="45"/>
       <c r="B51" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C51" s="25" t="s">
         <v>1</v>
@@ -1793,11 +1814,11 @@
         <v>4.18</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F51" s="23"/>
       <c r="G51" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1812,28 +1833,28 @@
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="45"/>
       <c r="B53" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C53" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F53" s="23"/>
       <c r="G53" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C54" s="24" t="s">
         <v>1</v>
@@ -1842,19 +1863,19 @@
         <v>2</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F54" s="23"/>
       <c r="G54" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C55" s="24" t="s">
         <v>1</v>
@@ -1863,11 +1884,11 @@
         <v>1.4</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1882,28 +1903,28 @@
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="45"/>
       <c r="B57" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C57" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F57" s="23"/>
       <c r="G57" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>1</v>
@@ -1912,19 +1933,19 @@
         <v>7.4</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F58" s="23"/>
       <c r="G58" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C59" s="24" t="s">
         <v>1</v>
@@ -1933,11 +1954,11 @@
         <v>22</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F59" s="23"/>
       <c r="G59" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -1952,28 +1973,28 @@
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="45"/>
       <c r="B61" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C61" s="25" t="s">
         <v>1</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F61" s="23"/>
       <c r="G61" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C62" s="25" t="s">
         <v>1</v>
@@ -1982,11 +2003,11 @@
         <v>22</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F62" s="23"/>
       <c r="G62" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -2001,28 +2022,28 @@
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="45"/>
       <c r="B64" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D64" s="23" t="s">
-        <v>37</v>
-      </c>
       <c r="E64" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F64" s="23"/>
       <c r="G64" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C65" s="32" t="s">
         <v>1</v>
@@ -2031,16 +2052,16 @@
         <v>22</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F65" s="30"/>
       <c r="G65" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B66" s="34"/>
       <c r="C66" s="35"/>
@@ -2052,7 +2073,7 @@
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="47"/>
       <c r="B67" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C67" s="36" t="s">
         <v>1</v>
@@ -2061,17 +2082,17 @@
         <v>750</v>
       </c>
       <c r="E67" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F67" s="34"/>
       <c r="G67" s="33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="47"/>
       <c r="B68" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C68" s="36" t="s">
         <v>1</v>
@@ -2080,17 +2101,17 @@
         <v>80</v>
       </c>
       <c r="E68" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F68" s="34"/>
       <c r="G68" s="33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="47"/>
       <c r="B69" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C69" s="36" t="s">
         <v>1</v>
@@ -2099,17 +2120,17 @@
         <v>900</v>
       </c>
       <c r="E69" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F69" s="34"/>
       <c r="G69" s="33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="47"/>
       <c r="B70" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C70" s="36" t="s">
         <v>1</v>
@@ -2118,17 +2139,17 @@
         <v>1200</v>
       </c>
       <c r="E70" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F70" s="34"/>
       <c r="G70" s="33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="47"/>
       <c r="B71" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C71" s="36" t="s">
         <v>1</v>
@@ -2137,17 +2158,17 @@
         <v>105</v>
       </c>
       <c r="E71" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F71" s="34"/>
       <c r="G71" s="33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="47"/>
       <c r="B72" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C72" s="36" t="s">
         <v>1</v>
@@ -2156,17 +2177,17 @@
         <v>12600</v>
       </c>
       <c r="E72" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F72" s="34"/>
       <c r="G72" s="33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="47"/>
       <c r="B73" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C73" s="36" t="s">
         <v>1</v>
@@ -2175,33 +2196,33 @@
         <v>3</v>
       </c>
       <c r="E73" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F73" s="34"/>
       <c r="G73" s="33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="48"/>
       <c r="B74" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C74" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E74" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F74" s="38"/>
       <c r="G74" s="37"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B75" s="34"/>
       <c r="C75" s="35"/>
@@ -2213,7 +2234,7 @@
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="47"/>
       <c r="B76" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C76" s="36" t="s">
         <v>1</v>
@@ -2222,17 +2243,17 @@
         <v>45</v>
       </c>
       <c r="E76" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F76" s="34"/>
       <c r="G76" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="47"/>
       <c r="B77" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C77" s="36" t="s">
         <v>1</v>
@@ -2241,17 +2262,17 @@
         <v>75</v>
       </c>
       <c r="E77" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F77" s="34"/>
       <c r="G77" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="47"/>
       <c r="B78" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C78" s="36" t="s">
         <v>1</v>
@@ -2260,17 +2281,17 @@
         <v>450</v>
       </c>
       <c r="E78" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F78" s="34"/>
       <c r="G78" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="47"/>
       <c r="B79" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C79" s="36" t="s">
         <v>1</v>
@@ -2279,11 +2300,11 @@
         <v>3600</v>
       </c>
       <c r="E79" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F79" s="34"/>
       <c r="G79" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
toward #27: finalized ECL fixes - needs debugging
</commit_message>
<xml_diff>
--- a/WF1_template.xlsx
+++ b/WF1_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAE48E6-D6FA-5248-B99F-D1B0D1C7EFD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B68869-3183-594E-86C6-1550DFA8A79F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="460" windowWidth="37520" windowHeight="27640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25280" yWindow="460" windowWidth="25920" windowHeight="27640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WF1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="141">
   <si>
     <t>ExpWorkflowVer</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>Symyx_96_well_0003</t>
-  </si>
-  <si>
-    <t>PyrrolidiniumIodide</t>
   </si>
   <si>
     <r>
@@ -331,9 +328,6 @@
     <t>Reagent5_item1_formulaconc</t>
   </si>
   <si>
-    <t>DMSO</t>
-  </si>
-  <si>
     <t>The workflow version of the experimental perovskite protocol.  Currently supported: 1, 1.1</t>
   </si>
   <si>
@@ -969,6 +963,9 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>AcNH3I</t>
   </si>
 </sst>
 </file>
@@ -1675,7 +1672,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1712,7 +1709,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1745,7 +1742,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H3" s="17"/>
     </row>
@@ -1767,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="77" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H4" s="17"/>
     </row>
@@ -1789,7 +1786,7 @@
         <v>27</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H5" s="27"/>
     </row>
@@ -1803,7 +1800,7 @@
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
       <c r="G6" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H6" s="32"/>
     </row>
@@ -1825,7 +1822,7 @@
         <v>96</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H7" s="32"/>
     </row>
@@ -1847,10 +1844,10 @@
         <v>14</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1869,10 +1866,10 @@
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1891,10 +1888,10 @@
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1915,7 +1912,7 @@
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H11" s="32"/>
     </row>
@@ -1937,7 +1934,7 @@
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H12" s="32"/>
     </row>
@@ -1959,13 +1956,13 @@
       </c>
       <c r="F13" s="70"/>
       <c r="G13" s="72" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H13" s="73"/>
     </row>
     <row r="14" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B14" s="35"/>
       <c r="C14" s="36"/>
@@ -1973,10 +1970,10 @@
       <c r="E14" s="35"/>
       <c r="F14" s="35"/>
       <c r="G14" s="37" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1992,13 +1989,13 @@
     <row r="16" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="34"/>
       <c r="B16" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="E16" s="35" t="s">
         <v>18</v>
@@ -2007,10 +2004,10 @@
         <v>26</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2026,7 +2023,7 @@
     <row r="18" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="34"/>
       <c r="B18" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="39" t="s">
         <v>1</v>
@@ -2041,10 +2038,10 @@
         <v>25</v>
       </c>
       <c r="G18" s="37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H18" s="60" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2052,7 +2049,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="36" t="s">
         <v>1</v>
@@ -2067,10 +2064,10 @@
         <v>0.1</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2078,7 +2075,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="36" t="s">
         <v>1</v>
@@ -2093,10 +2090,10 @@
         <v>3</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H20" s="38" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2112,13 +2109,13 @@
     <row r="22" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="34"/>
       <c r="B22" s="35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C22" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="E22" s="35" t="s">
         <v>18</v>
@@ -2127,10 +2124,10 @@
         <v>24</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H22" s="60" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2148,7 +2145,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C24" s="36" t="s">
         <v>1</v>
@@ -2163,10 +2160,10 @@
         <v>28</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H24" s="60" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2182,7 +2179,7 @@
     <row r="26" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="43"/>
       <c r="B26" s="44" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C26" s="47" t="s">
         <v>1</v>
@@ -2195,10 +2192,10 @@
         <v>57</v>
       </c>
       <c r="G26" s="45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H26" s="62" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2211,10 +2208,10 @@
       <c r="E27" s="35"/>
       <c r="F27" s="35"/>
       <c r="G27" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H27" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2230,7 +2227,7 @@
     <row r="29" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="34"/>
       <c r="B29" s="35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C29" s="39" t="s">
         <v>1</v>
@@ -2245,10 +2242,10 @@
         <v>41</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H29" s="38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2264,7 +2261,7 @@
     <row r="31" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="34"/>
       <c r="B31" s="35" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C31" s="39" t="s">
         <v>1</v>
@@ -2279,22 +2276,22 @@
         <v>42</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H31" s="38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34"/>
       <c r="B32" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="35">
-        <v>2.2799999999999998</v>
+        <v>0.75</v>
       </c>
       <c r="E32" s="35" t="s">
         <v>21</v>
@@ -2303,22 +2300,22 @@
         <v>3</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H32" s="38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="34"/>
       <c r="B33" s="35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="35">
-        <v>2.85</v>
+        <v>0.38</v>
       </c>
       <c r="E33" s="35" t="s">
         <v>21</v>
@@ -2327,7 +2324,7 @@
         <v>1.5</v>
       </c>
       <c r="G33" s="37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H33" s="38"/>
     </row>
@@ -2336,7 +2333,7 @@
         <v>15</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="36" t="s">
         <v>1</v>
@@ -2351,10 +2348,10 @@
         <v>75</v>
       </c>
       <c r="G34" s="37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H34" s="38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2362,7 +2359,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" s="36" t="s">
         <v>1</v>
@@ -2377,10 +2374,10 @@
         <v>450</v>
       </c>
       <c r="G35" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="H35" s="38" t="s">
         <v>99</v>
-      </c>
-      <c r="H35" s="38" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2388,7 +2385,7 @@
         <v>15</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="36" t="s">
         <v>1</v>
@@ -2403,10 +2400,10 @@
         <v>3600</v>
       </c>
       <c r="G36" s="37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H36" s="38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2422,7 +2419,7 @@
     <row r="38" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="34"/>
       <c r="B38" s="35" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C38" s="39" t="s">
         <v>1</v>
@@ -2437,20 +2434,20 @@
         <v>43</v>
       </c>
       <c r="G38" s="37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H38" s="38"/>
     </row>
     <row r="39" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="34"/>
       <c r="B39" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C39" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="35">
-        <v>4.18</v>
+        <v>5.84</v>
       </c>
       <c r="E39" s="35" t="s">
         <v>21</v>
@@ -2459,7 +2456,7 @@
         <v>6</v>
       </c>
       <c r="G39" s="37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H39" s="38"/>
     </row>
@@ -2478,7 +2475,7 @@
         <v>15</v>
       </c>
       <c r="B41" s="35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C41" s="36" t="s">
         <v>1</v>
@@ -2502,7 +2499,7 @@
         <v>15</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C42" s="36" t="s">
         <v>1</v>
@@ -2517,7 +2514,7 @@
         <v>2</v>
       </c>
       <c r="G42" s="37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H42" s="38"/>
     </row>
@@ -2526,7 +2523,7 @@
         <v>15</v>
       </c>
       <c r="B43" s="46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43" s="36" t="s">
         <v>1</v>
@@ -2541,7 +2538,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H43" s="38"/>
     </row>
@@ -2562,7 +2559,7 @@
         <v>15</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C45" s="36" t="s">
         <v>1</v>
@@ -2586,7 +2583,7 @@
         <v>15</v>
       </c>
       <c r="B46" s="46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C46" s="36" t="s">
         <v>1</v>
@@ -2601,7 +2598,7 @@
         <v>4.5</v>
       </c>
       <c r="G46" s="37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H46" s="38"/>
     </row>
@@ -2618,7 +2615,7 @@
     <row r="48" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="34"/>
       <c r="B48" s="35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C48" s="39" t="s">
         <v>1</v>
@@ -2650,7 +2647,7 @@
     <row r="50" spans="1:8" s="68" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="64"/>
       <c r="B50" s="65" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C50" s="66" t="s">
         <v>1</v>
@@ -2699,7 +2696,7 @@
         <v>750</v>
       </c>
       <c r="G52" s="51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H52" s="52"/>
     </row>
@@ -2721,7 +2718,7 @@
         <v>80</v>
       </c>
       <c r="G53" s="51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H53" s="52"/>
     </row>
@@ -2743,7 +2740,7 @@
         <v>900</v>
       </c>
       <c r="G54" s="51" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H54" s="52"/>
     </row>
@@ -2765,7 +2762,7 @@
         <v>1200</v>
       </c>
       <c r="G55" s="51" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H55" s="52"/>
     </row>
@@ -2787,10 +2784,10 @@
         <v>105</v>
       </c>
       <c r="G56" s="51" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H56" s="52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2811,10 +2808,10 @@
         <v>12600</v>
       </c>
       <c r="G57" s="51" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H57" s="52" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2835,10 +2832,10 @@
         <v>3</v>
       </c>
       <c r="G58" s="74" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H58" s="52" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2857,10 +2854,10 @@
       </c>
       <c r="F59" s="55"/>
       <c r="G59" s="58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H59" s="59" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2893,10 +2890,10 @@
         <v>45</v>
       </c>
       <c r="G61" s="51" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H61" s="75" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2917,10 +2914,10 @@
         <v>75</v>
       </c>
       <c r="G62" s="51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H62" s="75" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2941,10 +2938,10 @@
         <v>450</v>
       </c>
       <c r="G63" s="51" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H63" s="75" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2965,10 +2962,10 @@
         <v>3600</v>
       </c>
       <c r="G64" s="58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H64" s="76" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>